<commit_message>
Update the design specifications.
Signed-off-by: David Qiu <david@davidqiu.com>
</commit_message>
<xml_diff>
--- a/Documents/D-CUP Design Specifications.xlsx
+++ b/Documents/D-CUP Design Specifications.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7620"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Operations" sheetId="1" r:id="rId1"/>
     <sheet name="Registers" sheetId="2" r:id="rId2"/>
+    <sheet name="ALU Operations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="245">
   <si>
     <t>Operation List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2057,6 +2058,527 @@
   </si>
   <si>
     <t>Register List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arithmetic and Logic Unit Operation List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1+Input2 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1+Input2+Carry -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1-Input2 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1-Input2-Borrow -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Flags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output Flags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF, PF, ZF, NF, OF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PF, ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PF, ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF, ZF, NF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1-Input2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1 XOR Input2 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1 AND Input2 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1 OR Input2 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF, PF, ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF, PF, ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{: Input1} &lt;&lt; Input2[3:0] -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{CF, Input1, 0} &lt;&lt; Input2[3:0] -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0, Input1, CF} &gt;&gt; Input2[3:0] -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{Input1[0], Input1, CF} &gt;&gt; Input2[3:0] -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{Input1 :} &gt;&gt; Input2[3:0] -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1111</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1110</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1101</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1100</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0000</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0001</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ARRY</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0010</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0011</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0100</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0101</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0110</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0111</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1000</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1001</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1010</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1011</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2064,7 +2586,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2137,6 +2659,25 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="微软雅黑 Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="微软雅黑 Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2172,7 +2713,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2239,7 +2780,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2545,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -2562,16 +3112,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -3205,7 +3755,7 @@
       <c r="F28" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="9" t="s">
         <v>104</v>
       </c>
       <c r="H28" s="8" t="s">
@@ -3387,7 +3937,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -3400,12 +3950,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
@@ -3577,4 +4127,564 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A1" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the README.md, ALU module and documentation.
Signed-off-by: David Qiu <david@davidqiu.com>
</commit_message>
<xml_diff>
--- a/Documents/D-CUP Design Specifications.xlsx
+++ b/Documents/D-CUP Design Specifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Operations" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="252">
   <si>
     <t>Operation List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -26,18 +26,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Operand1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Operand2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Operand3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Opcode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -640,10 +628,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Arithmetic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -692,26 +676,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>E</t>
     </r>
@@ -782,38 +746,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SLR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>val3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>r1 &lt;- r2 shift left rotatory (val3 bit shift)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>r1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -834,10 +770,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>r1 &lt;- r2 shift right rotarory (val3 bit shift)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Logic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1823,6 +1755,27 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">IGHT </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
       <t>L</t>
     </r>
     <r>
@@ -1833,7 +1786,31 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">EFT </t>
+      <t>OGICAL</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">HIFT </t>
     </r>
     <r>
       <rPr>
@@ -1854,51 +1831,6 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>OTATORY</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">HIFT </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">IGHT </t>
     </r>
     <r>
@@ -1910,72 +1842,6 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>OGICAL</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">HIFT </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">IGHT </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
       <t>A</t>
     </r>
     <r>
@@ -1991,72 +1857,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">HIFT </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">IGHT </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>OTATORY</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Register List</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2125,10 +1925,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CF, PF, ZF, NF, OF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>XOR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2141,18 +1937,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PF, ZF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PF, ZF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CF, ZF, NF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2173,18 +1961,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CF, PF, ZF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CF, PF, ZF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{: Input1} &lt;&lt; Input2[3:0] -&gt; Output</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{CF, Input1, 0} &lt;&lt; Input2[3:0] -&gt; Output</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2194,10 +1970,6 @@
   </si>
   <si>
     <t>{Input1[0], Input1, CF} &gt;&gt; Input2[3:0] -&gt; Output</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{Input1 :} &gt;&gt; Input2[3:0] -&gt; Output</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2213,19 +1985,278 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0000</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0001</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ADD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ARRY</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0010</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0011</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0100</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0101</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>INC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>REASE</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1 &lt;- r2 + 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>1111</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>0110</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2238,15 +2269,15 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>1110</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1001</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2259,15 +2290,15 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>1101</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1010</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2280,15 +2311,15 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>1100</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1011</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2301,15 +2332,15 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>0000</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1100</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2322,60 +2353,15 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>0001</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ADD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ARRY</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1101</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2388,15 +2374,15 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>0010</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1110</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2409,15 +2395,71 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>0011</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>1111</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1+1 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF, ZF, NF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF, ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TRAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SFER</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2426,19 +2468,18 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>0100</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
+      <t>0111</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
@@ -2447,138 +2488,63 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>0101</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>0110</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>0111</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
       <t>1000</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1001</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1010</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>1011</t>
-    </r>
+    <t>ZF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TRAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SFER</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Special</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operand1
+(3 bits)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operand2
+(4 bits)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operand3
+(4 bits)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2586,7 +2552,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2678,6 +2644,32 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="微软雅黑 Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="微软雅黑 Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2713,7 +2705,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2774,23 +2766,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3095,8 +3108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -3112,795 +3125,790 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="33" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>184</v>
+        <v>17</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>185</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>168</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7" s="14" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>185</v>
+        <v>32</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>172</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B17" s="14" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B18" s="14" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B25" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="H28" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="B29" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>186</v>
+        <v>217</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>187</v>
+        <v>218</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="B31" s="13" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>111</v>
+        <v>220</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>112</v>
+        <v>221</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B34" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>121</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
@@ -3950,25 +3958,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -3976,13 +3984,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -3994,14 +4002,14 @@
       <c r="A5" s="18">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>147</v>
+      <c r="B5" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -4013,12 +4021,13 @@
       <c r="A7" s="18">
         <v>4</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>142</v>
-      </c>
+      <c r="B7" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
@@ -4030,13 +4039,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>131</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -4044,60 +4053,63 @@
         <v>7</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="18">
         <v>8</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>141</v>
-      </c>
+      <c r="B11" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="18">
         <v>9</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>143</v>
-      </c>
+      <c r="B12" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="18">
         <v>10</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>144</v>
-      </c>
+      <c r="B13" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="18">
         <v>11</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>150</v>
+      <c r="B14" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -4126,6 +4138,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4133,13 +4146,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
@@ -4147,536 +4160,537 @@
     <col min="10" max="10" width="48.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>201</v>
+        <v>181</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>182</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>201</v>
+        <v>181</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>182</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>201</v>
+        <v>181</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>182</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="F9" s="22">
+      <c r="C9" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="21">
         <v>0</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="G10" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>214</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>103</v>
+        <v>178</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="B12" s="13" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>214</v>
+        <v>192</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>104</v>
+        <v>227</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>123</v>
-      </c>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
       <c r="B13" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>214</v>
+        <v>192</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>193</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>186</v>
+        <v>228</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>214</v>
+        <v>192</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>193</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>187</v>
+        <v>229</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="B15" s="13" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>214</v>
+        <v>192</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>193</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>184</v>
+        <v>192</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>193</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>184</v>
+        <v>192</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>227</v>
+      <c r="B18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>